<commit_message>
Initial commit: SpecCon Holdings website with learnership application system
- Complete website for SpecCon Holdings training provider
- 47+ qualification pages across 7 SETAs
- Comprehensive learnership application form with assessments
- Speed typing, writing, math, and Excel skill tests
- Form validation and South African compliance
- Centralized modal system and value-adds popup
- Professional responsive design with Tailwind CSS

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Qualifications detail/Website Summary.xlsx
+++ b/Qualifications detail/Website Summary.xlsx
@@ -8,27 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\OneDrive - Speccon Holdings (Pty) Ltd\Websites\Speccon\Qualifications detail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B263CEBE-C9AC-4A37-AF20-446372DC23C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F744B0-10CD-4123-9DE5-15C2BE4D3D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="3" xr2:uid="{40E45FA6-4414-4754-8409-F6B849EFDC85}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{40E45FA6-4414-4754-8409-F6B849EFDC85}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet5" sheetId="8" r:id="rId1"/>
-    <sheet name="Qualifications" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="6" r:id="rId3"/>
-    <sheet name="Short Courses" sheetId="7" r:id="rId4"/>
-    <sheet name="Seta's" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId6"/>
-    <sheet name="Skills Programs" sheetId="3" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="9" r:id="rId2"/>
+    <sheet name="Qualifications" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="6" r:id="rId4"/>
+    <sheet name="Short Courses" sheetId="7" r:id="rId5"/>
+    <sheet name="Seta's" sheetId="5" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId7"/>
+    <sheet name="Skills Programs" sheetId="3" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Qualifications!$A$1:$N$52</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Sheet1!$A$1:$A$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Qualifications!$A$1:$N$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Sheet1!$A$1:$A$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="30" r:id="rId8"/>
+    <pivotCache cacheId="1" r:id="rId9"/>
   </pivotCaches>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -46,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="280">
   <si>
     <t>Qualification Name</t>
   </si>
@@ -1426,7 +1428,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -1493,12 +1495,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1548,7 +1546,505 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="160">
+  <dxfs count="326">
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center"/>
     </dxf>
@@ -3125,320 +3621,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ADF664B1-A43C-43FE-B2EB-F63EFE9566DF}" name="PivotTable2" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="A1:D12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="12">
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <items count="9">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <items count="44">
-        <item x="20"/>
-        <item x="25"/>
-        <item x="13"/>
-        <item x="21"/>
-        <item x="22"/>
-        <item x="14"/>
-        <item x="23"/>
-        <item x="24"/>
-        <item x="26"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="27"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="29"/>
-        <item x="12"/>
-        <item x="30"/>
-        <item x="31"/>
-        <item x="17"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="32"/>
-        <item x="36"/>
-        <item x="33"/>
-        <item x="34"/>
-        <item x="28"/>
-        <item x="37"/>
-        <item x="38"/>
-        <item x="39"/>
-        <item x="40"/>
-        <item x="41"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="42"/>
-        <item x="35"/>
-        <item x="43"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" numFmtId="15" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <items count="52">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="19"/>
-        <item x="37"/>
-        <item x="29"/>
-        <item x="27"/>
-        <item x="21"/>
-        <item x="30"/>
-        <item x="13"/>
-        <item x="38"/>
-        <item x="24"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="14"/>
-        <item x="5"/>
-        <item x="32"/>
-        <item x="31"/>
-        <item x="15"/>
-        <item x="22"/>
-        <item x="23"/>
-        <item x="20"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="34"/>
-        <item x="36"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="33"/>
-        <item x="28"/>
-        <item m="1" x="51"/>
-        <item x="39"/>
-        <item x="43"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="40"/>
-        <item x="41"/>
-        <item x="35"/>
-        <item x="44"/>
-        <item x="45"/>
-        <item x="46"/>
-        <item x="47"/>
-        <item x="48"/>
-        <item x="25"/>
-        <item x="26"/>
-        <item x="49"/>
-        <item x="42"/>
-        <item x="50"/>
-        <item x="12"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <items count="2">
-        <item x="0"/>
-        <item x="1"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <items count="102">
-        <item m="1" x="52"/>
-        <item m="1" x="53"/>
-        <item m="1" x="54"/>
-        <item m="1" x="55"/>
-        <item m="1" x="56"/>
-        <item m="1" x="57"/>
-        <item m="1" x="58"/>
-        <item m="1" x="59"/>
-        <item m="1" x="60"/>
-        <item m="1" x="61"/>
-        <item m="1" x="62"/>
-        <item m="1" x="63"/>
-        <item m="1" x="64"/>
-        <item m="1" x="65"/>
-        <item m="1" x="66"/>
-        <item m="1" x="67"/>
-        <item m="1" x="68"/>
-        <item m="1" x="69"/>
-        <item m="1" x="70"/>
-        <item m="1" x="71"/>
-        <item m="1" x="73"/>
-        <item m="1" x="75"/>
-        <item m="1" x="74"/>
-        <item m="1" x="76"/>
-        <item m="1" x="77"/>
-        <item m="1" x="72"/>
-        <item m="1" x="88"/>
-        <item m="1" x="80"/>
-        <item m="1" x="78"/>
-        <item m="1" x="81"/>
-        <item m="1" x="89"/>
-        <item m="1" x="83"/>
-        <item m="1" x="82"/>
-        <item m="1" x="85"/>
-        <item m="1" x="87"/>
-        <item m="1" x="79"/>
-        <item m="1" x="84"/>
-        <item m="1" x="90"/>
-        <item m="1" x="91"/>
-        <item m="1" x="92"/>
-        <item m="1" x="86"/>
-        <item m="1" x="93"/>
-        <item m="1" x="94"/>
-        <item m="1" x="95"/>
-        <item m="1" x="96"/>
-        <item m="1" x="97"/>
-        <item m="1" x="98"/>
-        <item m="1" x="99"/>
-        <item m="1" x="100"/>
-        <item m="1" x="101"/>
-        <item m="1" x="51"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="22"/>
-        <item x="24"/>
-        <item x="25"/>
-        <item x="26"/>
-        <item x="27"/>
-        <item x="28"/>
-        <item x="29"/>
-        <item x="30"/>
-        <item x="31"/>
-        <item x="32"/>
-        <item x="33"/>
-        <item x="34"/>
-        <item x="35"/>
-        <item x="36"/>
-        <item x="37"/>
-        <item x="38"/>
-        <item x="39"/>
-        <item x="40"/>
-        <item x="41"/>
-        <item x="42"/>
-        <item x="43"/>
-        <item x="44"/>
-        <item x="45"/>
-        <item x="46"/>
-        <item x="47"/>
-        <item x="48"/>
-        <item x="49"/>
-        <item x="50"/>
-        <item x="23"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="10">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="10"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count" fld="1" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="2">
-    <format dxfId="159">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="158">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{184D4575-2490-48B8-90D7-410E3634B462}" name="PivotTable1" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{184D4575-2490-48B8-90D7-410E3634B462}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A14:G65" firstHeaderRow="1" firstDataRow="1" firstDataCol="7"/>
   <pivotFields count="12">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -4169,19 +4352,19 @@
     <i/>
   </colItems>
   <formats count="152">
-    <format dxfId="157">
+    <format dxfId="323">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
     </format>
-    <format dxfId="156">
+    <format dxfId="322">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
     </format>
-    <format dxfId="155">
+    <format dxfId="321">
       <pivotArea field="10" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
     </format>
-    <format dxfId="154">
+    <format dxfId="320">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
     </format>
-    <format dxfId="153">
+    <format dxfId="319">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4199,7 +4382,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="152">
+    <format dxfId="318">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4217,7 +4400,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="151">
+    <format dxfId="317">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4235,7 +4418,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="150">
+    <format dxfId="316">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4253,7 +4436,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="149">
+    <format dxfId="315">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4271,7 +4454,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="148">
+    <format dxfId="314">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4289,7 +4472,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="147">
+    <format dxfId="313">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4307,7 +4490,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="146">
+    <format dxfId="312">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4325,7 +4508,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="145">
+    <format dxfId="311">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4343,7 +4526,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="144">
+    <format dxfId="310">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4361,7 +4544,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="143">
+    <format dxfId="309">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4379,7 +4562,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="142">
+    <format dxfId="308">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4397,7 +4580,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="141">
+    <format dxfId="307">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4415,7 +4598,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="140">
+    <format dxfId="306">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4433,7 +4616,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="139">
+    <format dxfId="305">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4451,7 +4634,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="138">
+    <format dxfId="304">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4469,7 +4652,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="137">
+    <format dxfId="303">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4487,7 +4670,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="136">
+    <format dxfId="302">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4505,7 +4688,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="135">
+    <format dxfId="301">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4523,7 +4706,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="134">
+    <format dxfId="300">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4541,7 +4724,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="133">
+    <format dxfId="299">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4559,7 +4742,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="132">
+    <format dxfId="298">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4577,7 +4760,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="131">
+    <format dxfId="297">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4595,7 +4778,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="130">
+    <format dxfId="296">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4613,7 +4796,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="129">
+    <format dxfId="295">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4631,7 +4814,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="128">
+    <format dxfId="294">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4649,7 +4832,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="127">
+    <format dxfId="293">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4667,7 +4850,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="126">
+    <format dxfId="292">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4685,7 +4868,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="125">
+    <format dxfId="291">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4703,7 +4886,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="124">
+    <format dxfId="290">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4721,7 +4904,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="123">
+    <format dxfId="289">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4739,7 +4922,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="122">
+    <format dxfId="288">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4757,7 +4940,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="121">
+    <format dxfId="287">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4775,7 +4958,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="120">
+    <format dxfId="286">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4793,7 +4976,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="119">
+    <format dxfId="285">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4811,7 +4994,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="118">
+    <format dxfId="284">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4829,7 +5012,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="117">
+    <format dxfId="283">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4847,7 +5030,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="116">
+    <format dxfId="282">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4865,7 +5048,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="115">
+    <format dxfId="281">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4883,7 +5066,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="114">
+    <format dxfId="280">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4901,7 +5084,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="113">
+    <format dxfId="279">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4919,7 +5102,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="112">
+    <format dxfId="278">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4937,7 +5120,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="111">
+    <format dxfId="277">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="4">
           <reference field="0" count="1" selected="0">
@@ -4955,7 +5138,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="110">
+    <format dxfId="276">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -4976,7 +5159,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="109">
+    <format dxfId="275">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -4997,7 +5180,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="108">
+    <format dxfId="274">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5018,7 +5201,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="107">
+    <format dxfId="273">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5039,7 +5222,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="106">
+    <format dxfId="272">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5060,7 +5243,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="105">
+    <format dxfId="271">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5081,7 +5264,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="104">
+    <format dxfId="270">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5102,7 +5285,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="103">
+    <format dxfId="269">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5123,7 +5306,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="102">
+    <format dxfId="268">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5144,7 +5327,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="101">
+    <format dxfId="267">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5165,7 +5348,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="100">
+    <format dxfId="266">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5186,7 +5369,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="99">
+    <format dxfId="265">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5207,7 +5390,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="98">
+    <format dxfId="264">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5228,7 +5411,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="97">
+    <format dxfId="263">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5249,7 +5432,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="96">
+    <format dxfId="262">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5270,7 +5453,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="95">
+    <format dxfId="261">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5291,7 +5474,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="94">
+    <format dxfId="260">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5312,7 +5495,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="93">
+    <format dxfId="259">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5333,7 +5516,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="92">
+    <format dxfId="258">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5354,7 +5537,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="91">
+    <format dxfId="257">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5375,7 +5558,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="90">
+    <format dxfId="256">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5396,7 +5579,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="89">
+    <format dxfId="255">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5417,7 +5600,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="88">
+    <format dxfId="254">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5438,7 +5621,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="87">
+    <format dxfId="253">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5459,7 +5642,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="86">
+    <format dxfId="252">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5480,7 +5663,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="85">
+    <format dxfId="251">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5501,7 +5684,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="84">
+    <format dxfId="250">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5522,7 +5705,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="83">
+    <format dxfId="249">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5543,7 +5726,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="82">
+    <format dxfId="248">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5564,7 +5747,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="81">
+    <format dxfId="247">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5585,7 +5768,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="80">
+    <format dxfId="246">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5606,7 +5789,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="79">
+    <format dxfId="245">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5627,7 +5810,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="78">
+    <format dxfId="244">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5648,7 +5831,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="77">
+    <format dxfId="243">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5669,7 +5852,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="76">
+    <format dxfId="242">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5690,7 +5873,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="75">
+    <format dxfId="241">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5711,7 +5894,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="74">
+    <format dxfId="240">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5732,7 +5915,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="73">
+    <format dxfId="239">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5753,7 +5936,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="72">
+    <format dxfId="238">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5774,7 +5957,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="71">
+    <format dxfId="237">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5795,7 +5978,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="70">
+    <format dxfId="236">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5816,7 +5999,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="69">
+    <format dxfId="235">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="5">
           <reference field="0" count="1" selected="0">
@@ -5837,7 +6020,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="68">
+    <format dxfId="234">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="6">
           <reference field="0" count="1" selected="0">
@@ -5861,7 +6044,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="67">
+    <format dxfId="233">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="6">
           <reference field="0" count="1" selected="0">
@@ -5885,7 +6068,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="66">
+    <format dxfId="232">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="6">
           <reference field="0" count="1" selected="0">
@@ -5909,7 +6092,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="65">
+    <format dxfId="231">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="6">
           <reference field="0" count="1" selected="0">
@@ -5933,7 +6116,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="64">
+    <format dxfId="230">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="6">
           <reference field="0" count="1" selected="0">
@@ -5957,7 +6140,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="63">
+    <format dxfId="229">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="6">
           <reference field="0" count="1" selected="0">
@@ -5981,7 +6164,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="62">
+    <format dxfId="228">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="6">
           <reference field="0" count="1" selected="0">
@@ -6005,7 +6188,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="61">
+    <format dxfId="227">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="6">
           <reference field="0" count="1" selected="0">
@@ -6029,7 +6212,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="60">
+    <format dxfId="226">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="6">
           <reference field="0" count="1" selected="0">
@@ -6053,7 +6236,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="59">
+    <format dxfId="225">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="6">
           <reference field="0" count="1" selected="0">
@@ -6077,7 +6260,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="58">
+    <format dxfId="224">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="6">
           <reference field="0" count="1" selected="0">
@@ -6101,7 +6284,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="57">
+    <format dxfId="223">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="6">
           <reference field="0" count="1" selected="0">
@@ -6125,7 +6308,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="56">
+    <format dxfId="222">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6152,7 +6335,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="55">
+    <format dxfId="221">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6179,7 +6362,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="54">
+    <format dxfId="220">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6206,7 +6389,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="53">
+    <format dxfId="219">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6233,7 +6416,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="52">
+    <format dxfId="218">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6260,7 +6443,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="51">
+    <format dxfId="217">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6287,7 +6470,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="50">
+    <format dxfId="216">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6314,7 +6497,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="49">
+    <format dxfId="215">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6341,7 +6524,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="48">
+    <format dxfId="214">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6368,7 +6551,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="47">
+    <format dxfId="213">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6395,7 +6578,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="46">
+    <format dxfId="212">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6422,7 +6605,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="45">
+    <format dxfId="211">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6449,7 +6632,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="44">
+    <format dxfId="210">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6476,7 +6659,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="43">
+    <format dxfId="209">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6503,7 +6686,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="42">
+    <format dxfId="208">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6530,7 +6713,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="41">
+    <format dxfId="207">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6557,7 +6740,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="40">
+    <format dxfId="206">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6584,7 +6767,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="39">
+    <format dxfId="205">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6611,7 +6794,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="38">
+    <format dxfId="204">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6638,7 +6821,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="37">
+    <format dxfId="203">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6665,7 +6848,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="36">
+    <format dxfId="202">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6692,7 +6875,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="35">
+    <format dxfId="201">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6719,7 +6902,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="34">
+    <format dxfId="200">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6746,7 +6929,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="33">
+    <format dxfId="199">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6773,7 +6956,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="32">
+    <format dxfId="198">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6800,7 +6983,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="31">
+    <format dxfId="197">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6827,7 +7010,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="30">
+    <format dxfId="196">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6854,7 +7037,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="29">
+    <format dxfId="195">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6881,7 +7064,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="28">
+    <format dxfId="194">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6908,7 +7091,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="27">
+    <format dxfId="193">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6935,7 +7118,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="26">
+    <format dxfId="192">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6962,7 +7145,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="25">
+    <format dxfId="191">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -6989,7 +7172,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="24">
+    <format dxfId="190">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -7016,7 +7199,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="23">
+    <format dxfId="189">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -7043,7 +7226,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="22">
+    <format dxfId="188">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -7070,7 +7253,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="21">
+    <format dxfId="187">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -7097,7 +7280,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="20">
+    <format dxfId="186">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -7124,7 +7307,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="19">
+    <format dxfId="185">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -7151,7 +7334,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="18">
+    <format dxfId="184">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -7178,7 +7361,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="17">
+    <format dxfId="183">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -7205,7 +7388,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="182">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -7232,7 +7415,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="15">
+    <format dxfId="181">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -7259,7 +7442,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="14">
+    <format dxfId="180">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -7286,7 +7469,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="179">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -7313,7 +7496,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="12">
+    <format dxfId="178">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -7340,7 +7523,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="11">
+    <format dxfId="177">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -7367,7 +7550,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="10">
+    <format dxfId="176">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -7394,7 +7577,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="175">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -7421,7 +7604,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="8">
+    <format dxfId="174">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -7448,7 +7631,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="173">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -7475,7 +7658,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="6">
+    <format dxfId="172">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="7">
           <reference field="0" count="1" selected="0">
@@ -7501,6 +7684,858 @@
           </reference>
         </references>
       </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ADF664B1-A43C-43FE-B2EB-F63EFE9566DF}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="A1:D12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="12">
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="9">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="44">
+        <item x="20"/>
+        <item x="25"/>
+        <item x="13"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="14"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="26"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="27"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="29"/>
+        <item x="12"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="17"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="32"/>
+        <item x="36"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="28"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="42"/>
+        <item x="35"/>
+        <item x="43"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" numFmtId="15" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="52">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="19"/>
+        <item x="37"/>
+        <item x="29"/>
+        <item x="27"/>
+        <item x="21"/>
+        <item x="30"/>
+        <item x="13"/>
+        <item x="38"/>
+        <item x="24"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="14"/>
+        <item x="5"/>
+        <item x="32"/>
+        <item x="31"/>
+        <item x="15"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="20"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="34"/>
+        <item x="36"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="33"/>
+        <item x="28"/>
+        <item m="1" x="51"/>
+        <item x="39"/>
+        <item x="43"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="35"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="49"/>
+        <item x="42"/>
+        <item x="50"/>
+        <item x="12"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="2">
+        <item x="0"/>
+        <item x="1"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="102">
+        <item m="1" x="52"/>
+        <item m="1" x="53"/>
+        <item m="1" x="54"/>
+        <item m="1" x="55"/>
+        <item m="1" x="56"/>
+        <item m="1" x="57"/>
+        <item m="1" x="58"/>
+        <item m="1" x="59"/>
+        <item m="1" x="60"/>
+        <item m="1" x="61"/>
+        <item m="1" x="62"/>
+        <item m="1" x="63"/>
+        <item m="1" x="64"/>
+        <item m="1" x="65"/>
+        <item m="1" x="66"/>
+        <item m="1" x="67"/>
+        <item m="1" x="68"/>
+        <item m="1" x="69"/>
+        <item m="1" x="70"/>
+        <item m="1" x="71"/>
+        <item m="1" x="73"/>
+        <item m="1" x="75"/>
+        <item m="1" x="74"/>
+        <item m="1" x="76"/>
+        <item m="1" x="77"/>
+        <item m="1" x="72"/>
+        <item m="1" x="88"/>
+        <item m="1" x="80"/>
+        <item m="1" x="78"/>
+        <item m="1" x="81"/>
+        <item m="1" x="89"/>
+        <item m="1" x="83"/>
+        <item m="1" x="82"/>
+        <item m="1" x="85"/>
+        <item m="1" x="87"/>
+        <item m="1" x="79"/>
+        <item m="1" x="84"/>
+        <item m="1" x="90"/>
+        <item m="1" x="91"/>
+        <item m="1" x="92"/>
+        <item m="1" x="86"/>
+        <item m="1" x="93"/>
+        <item m="1" x="94"/>
+        <item m="1" x="95"/>
+        <item m="1" x="96"/>
+        <item m="1" x="97"/>
+        <item m="1" x="98"/>
+        <item m="1" x="99"/>
+        <item m="1" x="100"/>
+        <item m="1" x="101"/>
+        <item m="1" x="51"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="23"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="10">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="10"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count" fld="1" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="2">
+    <format dxfId="325">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="324">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B4755F89-8A54-4B7E-8657-A153A04C029B}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="A2:B53" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
+  <pivotFields count="12">
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="9">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="5"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="31">
+        <item x="28"/>
+        <item x="30"/>
+        <item x="29"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="16"/>
+        <item x="14"/>
+        <item x="5"/>
+        <item x="25"/>
+        <item x="0"/>
+        <item x="8"/>
+        <item x="17"/>
+        <item x="12"/>
+        <item x="6"/>
+        <item x="20"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="13"/>
+        <item x="11"/>
+        <item x="19"/>
+        <item x="18"/>
+        <item x="7"/>
+        <item x="10"/>
+        <item x="22"/>
+        <item x="9"/>
+        <item x="15"/>
+        <item x="21"/>
+        <item x="3"/>
+        <item x="24"/>
+        <item x="23"/>
+        <item x="4"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="51">
+        <item x="3"/>
+        <item x="4"/>
+        <item x="23"/>
+        <item x="5"/>
+        <item x="0"/>
+        <item x="6"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="1"/>
+        <item x="7"/>
+        <item x="2"/>
+        <item x="11"/>
+        <item x="10"/>
+        <item x="22"/>
+        <item x="33"/>
+        <item x="12"/>
+        <item x="32"/>
+        <item x="31"/>
+        <item x="27"/>
+        <item x="21"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="20"/>
+        <item x="34"/>
+        <item x="30"/>
+        <item x="42"/>
+        <item x="37"/>
+        <item x="46"/>
+        <item x="16"/>
+        <item x="47"/>
+        <item x="38"/>
+        <item x="50"/>
+        <item x="49"/>
+        <item x="48"/>
+        <item x="13"/>
+        <item x="40"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="43"/>
+        <item x="18"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="17"/>
+        <item x="19"/>
+        <item x="24"/>
+        <item x="36"/>
+        <item x="39"/>
+        <item x="35"/>
+        <item x="41"/>
+        <item x="26"/>
+        <item x="25"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="6">
+        <item x="5"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" numFmtId="15" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="52">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="19"/>
+        <item x="37"/>
+        <item x="29"/>
+        <item x="27"/>
+        <item x="21"/>
+        <item x="30"/>
+        <item x="13"/>
+        <item x="38"/>
+        <item x="24"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="14"/>
+        <item x="5"/>
+        <item x="32"/>
+        <item x="31"/>
+        <item x="15"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="20"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="34"/>
+        <item x="36"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="33"/>
+        <item x="28"/>
+        <item m="1" x="51"/>
+        <item x="39"/>
+        <item x="43"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="35"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="49"/>
+        <item x="42"/>
+        <item x="50"/>
+        <item x="12"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="2">
+        <item x="0"/>
+        <item x="1"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="102">
+        <item m="1" x="52"/>
+        <item m="1" x="53"/>
+        <item m="1" x="54"/>
+        <item m="1" x="55"/>
+        <item m="1" x="56"/>
+        <item m="1" x="57"/>
+        <item m="1" x="58"/>
+        <item m="1" x="59"/>
+        <item m="1" x="60"/>
+        <item m="1" x="61"/>
+        <item m="1" x="62"/>
+        <item m="1" x="63"/>
+        <item m="1" x="64"/>
+        <item m="1" x="65"/>
+        <item m="1" x="66"/>
+        <item m="1" x="67"/>
+        <item m="1" x="68"/>
+        <item m="1" x="69"/>
+        <item m="1" x="70"/>
+        <item m="1" x="71"/>
+        <item m="1" x="73"/>
+        <item m="1" x="75"/>
+        <item m="1" x="74"/>
+        <item m="1" x="76"/>
+        <item m="1" x="77"/>
+        <item m="1" x="72"/>
+        <item m="1" x="88"/>
+        <item m="1" x="80"/>
+        <item m="1" x="78"/>
+        <item m="1" x="81"/>
+        <item m="1" x="89"/>
+        <item m="1" x="83"/>
+        <item m="1" x="82"/>
+        <item m="1" x="85"/>
+        <item m="1" x="87"/>
+        <item m="1" x="79"/>
+        <item m="1" x="84"/>
+        <item m="1" x="90"/>
+        <item m="1" x="91"/>
+        <item m="1" x="92"/>
+        <item m="1" x="86"/>
+        <item m="1" x="93"/>
+        <item m="1" x="94"/>
+        <item m="1" x="95"/>
+        <item m="1" x="96"/>
+        <item m="1" x="97"/>
+        <item m="1" x="98"/>
+        <item m="1" x="99"/>
+        <item m="1" x="100"/>
+        <item m="1" x="101"/>
+        <item m="1" x="51"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="23"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="9"/>
+    <field x="10"/>
+  </rowFields>
+  <rowItems count="51">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="4"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="5"/>
+      <x/>
+    </i>
+    <i>
+      <x v="6"/>
+      <x/>
+    </i>
+    <i>
+      <x v="7"/>
+      <x/>
+    </i>
+    <i>
+      <x v="8"/>
+      <x/>
+    </i>
+    <i>
+      <x v="9"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="10"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="11"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="12"/>
+      <x/>
+    </i>
+    <i>
+      <x v="13"/>
+      <x/>
+    </i>
+    <i>
+      <x v="14"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="15"/>
+      <x/>
+    </i>
+    <i>
+      <x v="16"/>
+      <x/>
+    </i>
+    <i>
+      <x v="17"/>
+      <x/>
+    </i>
+    <i>
+      <x v="18"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="19"/>
+      <x/>
+    </i>
+    <i>
+      <x v="20"/>
+      <x/>
+    </i>
+    <i>
+      <x v="21"/>
+      <x/>
+    </i>
+    <i>
+      <x v="22"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="23"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="24"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="25"/>
+      <x/>
+    </i>
+    <i>
+      <x v="26"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="27"/>
+      <x/>
+    </i>
+    <i>
+      <x v="28"/>
+      <x/>
+    </i>
+    <i>
+      <x v="29"/>
+      <x/>
+    </i>
+    <i>
+      <x v="30"/>
+      <x/>
+    </i>
+    <i>
+      <x v="32"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="33"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="34"/>
+      <x/>
+    </i>
+    <i>
+      <x v="35"/>
+      <x/>
+    </i>
+    <i>
+      <x v="36"/>
+      <x/>
+    </i>
+    <i>
+      <x v="37"/>
+      <x/>
+    </i>
+    <i>
+      <x v="38"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="39"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="40"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="41"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="42"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="43"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="44"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="45"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="46"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="47"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="48"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="49"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="50"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="51"/>
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <formats count="4">
+    <format dxfId="168">
+      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0"/>
+    </format>
+    <format dxfId="169">
+      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0"/>
+    </format>
+    <format dxfId="170">
+      <pivotArea field="10" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    </format>
+    <format dxfId="171">
+      <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
   </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -7815,14 +8850,15 @@
   <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="14" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I26" sqref="I26"/>
+      <pane ySplit="14" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G65" sqref="A13:G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7265625" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.7265625" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.36328125" style="8" bestFit="1" customWidth="1"/>
@@ -7833,16 +8869,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>260</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="31" t="s">
         <v>72</v>
       </c>
       <c r="D1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -7859,11 +8895,11 @@
       <c r="A3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="33">
+      <c r="B3" s="8">
         <v>12</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8">
         <v>12</v>
       </c>
     </row>
@@ -7871,11 +8907,11 @@
       <c r="A4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="33">
+      <c r="B4" s="8">
         <v>1</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33">
+      <c r="C4" s="8"/>
+      <c r="D4" s="8">
         <v>1</v>
       </c>
     </row>
@@ -7883,11 +8919,11 @@
       <c r="A5" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8">
         <v>1</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="8">
         <v>1</v>
       </c>
     </row>
@@ -7895,11 +8931,11 @@
       <c r="A6" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8">
         <v>5</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6" s="8">
         <v>5</v>
       </c>
     </row>
@@ -7907,11 +8943,11 @@
       <c r="A7" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8">
         <v>1</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="8">
         <v>1</v>
       </c>
     </row>
@@ -7919,13 +8955,13 @@
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="33">
+      <c r="B8" s="8">
         <v>4</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="8">
         <v>3</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="8">
         <v>7</v>
       </c>
     </row>
@@ -7933,13 +8969,13 @@
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="33">
+      <c r="B9" s="8">
         <v>8</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="8">
         <v>7</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="8">
         <v>15</v>
       </c>
     </row>
@@ -7947,11 +8983,11 @@
       <c r="A10" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8">
         <v>1</v>
       </c>
-      <c r="D10" s="33">
+      <c r="D10" s="8">
         <v>1</v>
       </c>
     </row>
@@ -7959,11 +8995,11 @@
       <c r="A11" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8">
         <v>8</v>
       </c>
-      <c r="D11" s="33">
+      <c r="D11" s="8">
         <v>8</v>
       </c>
     </row>
@@ -7971,41 +9007,40 @@
       <c r="A12" t="s">
         <v>170</v>
       </c>
-      <c r="B12" s="33">
+      <c r="B12" s="8">
         <v>25</v>
       </c>
-      <c r="C12" s="33">
+      <c r="C12" s="8">
         <v>26</v>
       </c>
-      <c r="D12" s="33">
+      <c r="D12" s="8">
         <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="D14" s="34" t="s">
+      <c r="D14" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="34" t="s">
+      <c r="E14" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="34" t="s">
+      <c r="F14" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="G14" s="34" t="s">
+      <c r="G14" s="32" t="s">
         <v>4</v>
       </c>
     </row>
@@ -9062,6 +10097,450 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{950195F9-D729-411E-BC12-68F73D25AA9D}">
+  <dimension ref="A1:G53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="70" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="14.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>190</v>
+      </c>
+      <c r="B10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>183</v>
+      </c>
+      <c r="B12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>191</v>
+      </c>
+      <c r="B14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>174</v>
+      </c>
+      <c r="B15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>175</v>
+      </c>
+      <c r="B16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>184</v>
+      </c>
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>176</v>
+      </c>
+      <c r="B18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>185</v>
+      </c>
+      <c r="B21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>192</v>
+      </c>
+      <c r="B22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>193</v>
+      </c>
+      <c r="B23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>194</v>
+      </c>
+      <c r="B24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>186</v>
+      </c>
+      <c r="B25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>187</v>
+      </c>
+      <c r="B26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>188</v>
+      </c>
+      <c r="B27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>177</v>
+      </c>
+      <c r="B30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>178</v>
+      </c>
+      <c r="B31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>198</v>
+      </c>
+      <c r="B35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>179</v>
+      </c>
+      <c r="B36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>180</v>
+      </c>
+      <c r="B37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>181</v>
+      </c>
+      <c r="B38" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>182</v>
+      </c>
+      <c r="B39" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>88</v>
+      </c>
+      <c r="B40" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>89</v>
+      </c>
+      <c r="B41" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>199</v>
+      </c>
+      <c r="B43" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>200</v>
+      </c>
+      <c r="B44" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>201</v>
+      </c>
+      <c r="B45" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>202</v>
+      </c>
+      <c r="B46" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>203</v>
+      </c>
+      <c r="B47" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>195</v>
+      </c>
+      <c r="B48" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>196</v>
+      </c>
+      <c r="B49" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>204</v>
+      </c>
+      <c r="B50" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>197</v>
+      </c>
+      <c r="B51" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>205</v>
+      </c>
+      <c r="B52" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>259</v>
+      </c>
+      <c r="B53" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B1EBB41-4362-403B-BC69-F6CAF2FDC970}">
   <dimension ref="A1:N52"/>
   <sheetViews>
@@ -11346,7 +12825,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19966282-678A-4B80-9453-7008044553FE}">
   <dimension ref="A1:A50"/>
   <sheetViews>
@@ -11666,12 +13145,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3784F58-4F6C-4F52-8EC5-988CF29D9330}">
   <dimension ref="A2:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11757,8 +13236,7 @@
       <c r="A12" t="s">
         <v>270</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="30" t="s">
         <v>167</v>
       </c>
     </row>
@@ -11860,7 +13338,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB907B53-C700-4F7C-8241-6A33C9AAD572}">
   <dimension ref="A1:A8"/>
   <sheetViews>
@@ -11928,7 +13406,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{384E9258-10FF-434A-85A2-6843DB843905}">
   <dimension ref="A2:C16"/>
   <sheetViews>
@@ -12147,7 +13625,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{332DD47C-E2BB-4A2C-9B91-6F57C7FB6D06}">
   <dimension ref="A1:K3"/>
   <sheetViews>

</xml_diff>